<commit_message>
revised scripts for sankey
</commit_message>
<xml_diff>
--- a/PythonResources/RunCases/sankey_modelica.xlsx
+++ b/PythonResources/RunCases/sankey_modelica.xlsx
@@ -466,7 +466,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>10729179.656</v>
+        <v>10612736.799</v>
       </c>
     </row>
     <row r="3">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>9361576.076445993</v>
+        <v>9361383.787897468</v>
       </c>
     </row>
     <row r="4">
@@ -496,7 +496,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>427117.5129158389</v>
+        <v>427071.2710208746</v>
       </c>
     </row>
     <row r="5">
@@ -511,7 +511,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>168391.5592462147</v>
+        <v>168391.0278618892</v>
       </c>
     </row>
     <row r="6">
@@ -526,7 +526,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1125.297661889782</v>
+        <v>1125.222010135986</v>
       </c>
     </row>
     <row r="7">
@@ -541,7 +541,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>4751350.922267174</v>
+        <v>4762481.516371373</v>
       </c>
     </row>
     <row r="8">
@@ -556,7 +556,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>3139053.66500762</v>
+        <v>3134861.941707576</v>
       </c>
     </row>
     <row r="9">
@@ -571,7 +571,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>36866.18578081422</v>
+        <v>37363.77303307541</v>
       </c>
     </row>
     <row r="10">
@@ -586,7 +586,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1710739.295897347</v>
+        <v>1707840.615235701</v>
       </c>
     </row>
     <row r="11">
@@ -601,7 +601,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>2925490.740262752</v>
+        <v>2916925.832670349</v>
       </c>
     </row>
     <row r="12">
@@ -616,7 +616,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>9626644.850775661</v>
+        <v>9632461.800901605</v>
       </c>
     </row>
     <row r="13">
@@ -631,7 +631,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>12142727.90108603</v>
+        <v>12171623.16534381</v>
       </c>
     </row>
     <row r="14">
@@ -646,7 +646,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>3585258.514076063</v>
+        <v>3576208.440460043</v>
       </c>
     </row>
     <row r="15">
@@ -661,7 +661,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>35429.79293703954</v>
+        <v>48166.72185764778</v>
       </c>
     </row>
     <row r="16">
@@ -676,7 +676,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>8200189.726678429</v>
+        <v>8191767.866063803</v>
       </c>
     </row>
     <row r="17">
@@ -691,7 +691,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>387895.3139308491</v>
+        <v>390241.5577952634</v>
       </c>
     </row>
     <row r="18">
@@ -706,7 +706,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>15915196.58823537</v>
+        <v>15918445.0859807</v>
       </c>
     </row>
     <row r="19">
@@ -721,7 +721,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>26792.88601109157</v>
+        <v>25570.9059762565</v>
       </c>
     </row>
     <row r="20">
@@ -736,7 +736,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>8102663.769605235</v>
+        <v>8063011.671290446</v>
       </c>
     </row>
     <row r="21">
@@ -751,7 +751,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1077311.134359977</v>
+        <v>1076708.486683669</v>
       </c>
     </row>
     <row r="22">
@@ -766,7 +766,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>9204871.622685794</v>
+        <v>9222530.238275034</v>
       </c>
     </row>
     <row r="23">
@@ -781,7 +781,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>16910812.62820918</v>
+        <v>16911643.5345532</v>
       </c>
     </row>
     <row r="24">
@@ -796,7 +796,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>10057849.38217836</v>
+        <v>10056633.80555829</v>
       </c>
     </row>
     <row r="25">
@@ -811,7 +811,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>4864741.803249995</v>
+        <v>4864814.490741099</v>
       </c>
     </row>
   </sheetData>
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2634146.48</v>
+        <v>2632858.689</v>
       </c>
     </row>
     <row r="3">
@@ -877,7 +877,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3503781.904898992</v>
+        <v>3503815.793273349</v>
       </c>
     </row>
     <row r="4">
@@ -892,7 +892,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>84920.09380192525</v>
+        <v>84927.53610156653</v>
       </c>
     </row>
     <row r="5">
@@ -907,7 +907,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>90141.22606810112</v>
+        <v>90142.40046959631</v>
       </c>
     </row>
     <row r="6">
@@ -922,7 +922,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>430.6307944614983</v>
+        <v>430.7349768272641</v>
       </c>
     </row>
     <row r="7">
@@ -937,7 +937,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>2267813.147636606</v>
+        <v>2267835.727646634</v>
       </c>
     </row>
     <row r="8">
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>422653.6224848045</v>
+        <v>422996.1914057396</v>
       </c>
     </row>
     <row r="9">
@@ -967,7 +967,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>4931.454988933623</v>
+        <v>4906.550578521911</v>
       </c>
     </row>
     <row r="10">
@@ -982,7 +982,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1207747.532610571</v>
+        <v>1202965.617614802</v>
       </c>
     </row>
     <row r="11">
@@ -997,7 +997,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1635905.761785873</v>
+        <v>1633985.851825688</v>
       </c>
     </row>
     <row r="12">
@@ -1012,7 +1012,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>70234.02712835938</v>
+        <v>70729.94895657552</v>
       </c>
     </row>
     <row r="13">
@@ -1027,7 +1027,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>82366.65768125493</v>
+        <v>83529.94538636699</v>
       </c>
     </row>
     <row r="14">
@@ -1042,7 +1042,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1992026.964050616</v>
+        <v>1993490.370876481</v>
       </c>
     </row>
     <row r="15">
@@ -1057,7 +1057,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>125.8318707809883</v>
+        <v>134.0736238995695</v>
       </c>
     </row>
     <row r="16">
@@ -1072,7 +1072,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4575017.573129999</v>
+        <v>4574555.5783332</v>
       </c>
     </row>
     <row r="17">
@@ -1087,7 +1087,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>47415.23629906756</v>
+        <v>47037.37409917702</v>
       </c>
     </row>
     <row r="18">
@@ -1102,7 +1102,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>861997.680670761</v>
+        <v>861371.2632042464</v>
       </c>
     </row>
     <row r="19">
@@ -1117,7 +1117,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>26790.8817163299</v>
+        <v>25570.6814868186</v>
       </c>
     </row>
     <row r="20">
@@ -1132,7 +1132,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>84840.37763310559</v>
+        <v>84848.62563179298</v>
       </c>
     </row>
     <row r="21">
@@ -1147,7 +1147,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>471473.2910354374</v>
+        <v>470922.3242761792</v>
       </c>
     </row>
     <row r="22">
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>6831205.416878411</v>
+        <v>6832519.15028209</v>
       </c>
     </row>
     <row r="23">
@@ -1177,7 +1177,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>846872.668154462</v>
+        <v>846992.9392212338</v>
       </c>
     </row>
     <row r="24">
@@ -1192,7 +1192,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>7167159.264161864</v>
+        <v>7167326.040527486</v>
       </c>
     </row>
     <row r="25">
@@ -1207,7 +1207,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2030912.605535726</v>
+        <v>2030911.169037429</v>
       </c>
     </row>
   </sheetData>
@@ -1258,7 +1258,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>3643850.713</v>
+        <v>3611313.025</v>
       </c>
     </row>
     <row r="3">
@@ -1273,7 +1273,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>2503956.179142086</v>
+        <v>2503991.560105643</v>
       </c>
     </row>
     <row r="4">
@@ -1288,7 +1288,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>137480.1096873312</v>
+        <v>137509.8244841086</v>
       </c>
     </row>
     <row r="5">
@@ -1303,7 +1303,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>36926.75972342549</v>
+        <v>36926.52602441507</v>
       </c>
     </row>
     <row r="6">
@@ -1318,7 +1318,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>303.9622952749389</v>
+        <v>303.7396682196943</v>
       </c>
     </row>
     <row r="7">
@@ -1333,7 +1333,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1013317.749575402</v>
+        <v>1013057.410638321</v>
       </c>
     </row>
     <row r="8">
@@ -1348,7 +1348,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>908304.5308464034</v>
+        <v>895009.8610308161</v>
       </c>
     </row>
     <row r="9">
@@ -1363,7 +1363,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17651.71998621125</v>
+        <v>17362.58003323062</v>
       </c>
     </row>
     <row r="10">
@@ -1378,7 +1378,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>296125.6889772483</v>
+        <v>300190.6254883407</v>
       </c>
     </row>
     <row r="11">
@@ -1393,7 +1393,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>552365.4746429928</v>
+        <v>555922.9406147172</v>
       </c>
     </row>
     <row r="12">
@@ -1408,7 +1408,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>3469394.923596887</v>
+        <v>3427843.326436596</v>
       </c>
     </row>
     <row r="13">
@@ -1423,7 +1423,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>4327444.612167097</v>
+        <v>4276221.634823779</v>
       </c>
     </row>
     <row r="14">
@@ -1438,7 +1438,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>653863.0414033598</v>
+        <v>657593.8075766476</v>
       </c>
     </row>
     <row r="15">
@@ -1468,7 +1468,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3050165.161679783</v>
+        <v>3007150.016121518</v>
       </c>
     </row>
     <row r="17">
@@ -1483,7 +1483,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>121357.5708597995</v>
+        <v>120028.7507701389</v>
       </c>
     </row>
     <row r="18">
@@ -1498,7 +1498,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>5093286.396112598</v>
+        <v>5095320.870198407</v>
       </c>
     </row>
     <row r="19">
@@ -1528,7 +1528,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3624725.618509852</v>
+        <v>3614326.961078656</v>
       </c>
     </row>
     <row r="21">
@@ -1543,7 +1543,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>394898.1215747712</v>
+        <v>392742.8991128182</v>
       </c>
     </row>
     <row r="22">
@@ -1558,7 +1558,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1356622.64773764</v>
+        <v>1350821.221885394</v>
       </c>
     </row>
     <row r="23">
@@ -1573,7 +1573,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>5554871.343789381</v>
+        <v>5554481.332280847</v>
       </c>
     </row>
     <row r="24">
@@ -1588,7 +1588,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1448380.300067266</v>
+        <v>1447241.690690052</v>
       </c>
     </row>
     <row r="25">
@@ -1603,7 +1603,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1383079.46818868</v>
+        <v>1383142.843993499</v>
       </c>
     </row>
   </sheetData>
@@ -1654,7 +1654,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>3043335.517</v>
+        <v>2985749.657</v>
       </c>
     </row>
     <row r="3">
@@ -1669,7 +1669,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1936723.710034952</v>
+        <v>1936567.557996062</v>
       </c>
     </row>
     <row r="4">
@@ -1684,7 +1684,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>132180.9016869731</v>
+        <v>132145.0986409418</v>
       </c>
     </row>
     <row r="5">
@@ -1699,7 +1699,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>18712.53551253272</v>
+        <v>18710.80647416027</v>
       </c>
     </row>
     <row r="6">
@@ -1714,7 +1714,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>217.6927870679056</v>
+        <v>217.8549673544717</v>
       </c>
     </row>
     <row r="7">
@@ -1729,7 +1729,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>939347.7584247421</v>
+        <v>946717.9214573825</v>
       </c>
     </row>
     <row r="8">
@@ -1744,7 +1744,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1416406.942424569</v>
+        <v>1431970.464481312</v>
       </c>
     </row>
     <row r="9">
@@ -1759,7 +1759,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>8725.324280851006</v>
+        <v>9574.845410824915</v>
       </c>
     </row>
     <row r="10">
@@ -1774,7 +1774,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>67826.78274379398</v>
+        <v>68165.67793764456</v>
       </c>
     </row>
     <row r="11">
@@ -1789,7 +1789,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1.267662109492715e-17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -1804,7 +1804,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>4821702.557727703</v>
+        <v>4876128.929057013</v>
       </c>
     </row>
     <row r="13">
@@ -1819,7 +1819,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>6287948.843599956</v>
+        <v>6374173.245414898</v>
       </c>
     </row>
     <row r="14">
@@ -1834,7 +1834,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1157.771084162326</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -1849,7 +1849,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>35303.96106625855</v>
+        <v>48032.64823374821</v>
       </c>
     </row>
     <row r="16">
@@ -1864,7 +1864,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>144926.5956183833</v>
+        <v>177464.7296604221</v>
       </c>
     </row>
     <row r="17">
@@ -1879,7 +1879,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>99753.40783067947</v>
+        <v>102803.3748363527</v>
       </c>
     </row>
     <row r="18">
@@ -1894,7 +1894,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>7588645.24566276</v>
+        <v>7576664.279569159</v>
       </c>
     </row>
     <row r="19">
@@ -1909,7 +1909,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>2.004294761669382</v>
+        <v>0.2244894378993121</v>
       </c>
     </row>
     <row r="20">
@@ -1924,7 +1924,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>2862371.45822611</v>
+        <v>2839789.764353736</v>
       </c>
     </row>
     <row r="21">
@@ -1939,7 +1939,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>88442.51924432344</v>
+        <v>89883.38501352376</v>
       </c>
     </row>
     <row r="22">
@@ -1954,7 +1954,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>100571.0879230125</v>
+        <v>113923.2334113341</v>
       </c>
     </row>
     <row r="23">
@@ -1969,7 +1969,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>7981668.781877534</v>
+        <v>7982391.865773327</v>
       </c>
     </row>
     <row r="24">
@@ -1984,7 +1984,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>460944.8796589198</v>
+        <v>461273.8499141681</v>
       </c>
     </row>
     <row r="25">
@@ -1999,7 +1999,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>803143.5558708379</v>
+        <v>803194.6726352386</v>
       </c>
     </row>
   </sheetData>
@@ -2050,7 +2050,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1407846.946</v>
+        <v>1382815.428</v>
       </c>
     </row>
     <row r="3">
@@ -2065,7 +2065,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1417114.282369961</v>
+        <v>1417008.876522413</v>
       </c>
     </row>
     <row r="4">
@@ -2080,7 +2080,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>72536.40773960931</v>
+        <v>72488.81179425762</v>
       </c>
     </row>
     <row r="5">
@@ -2095,7 +2095,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>22611.03794215544</v>
+        <v>22611.29489371755</v>
       </c>
     </row>
     <row r="6">
@@ -2110,7 +2110,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>173.0117850854393</v>
+        <v>172.8923977345558</v>
       </c>
     </row>
     <row r="7">
@@ -2125,7 +2125,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>530872.2666304231</v>
+        <v>534870.456629036</v>
       </c>
     </row>
     <row r="8">
@@ -2140,7 +2140,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>391688.5692518435</v>
+        <v>384885.4247897079</v>
       </c>
     </row>
     <row r="9">
@@ -2155,7 +2155,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>5557.686524818335</v>
+        <v>5519.797010497965</v>
       </c>
     </row>
     <row r="10">
@@ -2170,7 +2170,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>139039.2915657346</v>
+        <v>136518.6941949135</v>
       </c>
     </row>
     <row r="11">
@@ -2185,7 +2185,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>737172.1260784965</v>
+        <v>726971.4753909551</v>
       </c>
     </row>
     <row r="12">
@@ -2200,7 +2200,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1265283.007311376</v>
+        <v>1257730.313854475</v>
       </c>
     </row>
     <row r="13">
@@ -2215,7 +2215,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>1444917.474847137</v>
+        <v>1437667.017306131</v>
       </c>
     </row>
     <row r="14">
@@ -2230,7 +2230,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>938151.599252105</v>
+        <v>925067.9555927777</v>
       </c>
     </row>
     <row r="15">
@@ -2260,7 +2260,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>429996.194219622</v>
+        <v>432531.2941499744</v>
       </c>
     </row>
     <row r="17">
@@ -2275,7 +2275,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>119363.3143472756</v>
+        <v>120359.2339824744</v>
       </c>
     </row>
     <row r="18">
@@ -2290,7 +2290,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>2371162.48857627</v>
+        <v>2385057.560746178</v>
       </c>
     </row>
     <row r="19">
@@ -2320,7 +2320,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1530687.030766852</v>
+        <v>1524032.102866277</v>
       </c>
     </row>
     <row r="21">
@@ -2335,7 +2335,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>122486.941324751</v>
+        <v>123150.858414662</v>
       </c>
     </row>
     <row r="22">
@@ -2350,7 +2350,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>916361.990800313</v>
+        <v>925174.3813804917</v>
       </c>
     </row>
     <row r="23">
@@ -2365,7 +2365,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>2527399.834387797</v>
+        <v>2527777.39727779</v>
       </c>
     </row>
     <row r="24">
@@ -2380,7 +2380,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>981364.938290313</v>
+        <v>980792.2244265833</v>
       </c>
     </row>
     <row r="25">
@@ -2395,7 +2395,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>647606.1736547512</v>
+        <v>647565.8050749324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>